<commit_message>
more experiments and gui prototype
</commit_message>
<xml_diff>
--- a/results/5000/v2/resultsSummaryBagOfWords5000.xlsx
+++ b/results/5000/v2/resultsSummaryBagOfWords5000.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programowanie\python\przetwarzanieJezykaNaturalnego\projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programowanie\python\przetwarzanieJezykaNaturalnego\projekt\results\5000\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8784883B-0DA1-4B82-90F9-1B87F6BACFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE96A10-4E7C-4936-BD80-C7D88769F906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-21720" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="200">
   <si>
     <t>Model</t>
   </si>
@@ -614,6 +627,12 @@
   </si>
   <si>
     <t>{'C': 2.0, 'solver': 'saga', 'max_iter': 10000, 'tol': 0.0001}</t>
+  </si>
+  <si>
+    <t>Średnia</t>
+  </si>
+  <si>
+    <t>MAX</t>
   </si>
 </sst>
 </file>
@@ -976,9 +995,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G190"/>
+  <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5356,6 +5377,32 @@
         <v>0.87582112000000001</v>
       </c>
     </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E192" t="s">
+        <v>198</v>
+      </c>
+      <c r="F192">
+        <f>AVERAGE(F2:F190)</f>
+        <v>0.83396984126984175</v>
+      </c>
+      <c r="G192">
+        <f>AVERAGE(G2:G190)</f>
+        <v>0.90744747068783016</v>
+      </c>
+    </row>
+    <row r="193" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E193" t="s">
+        <v>199</v>
+      </c>
+      <c r="F193">
+        <f>MAX(F2:F190)</f>
+        <v>0.85809999999999997</v>
+      </c>
+      <c r="G193">
+        <f>MAX(G2:G190)</f>
+        <v>0.93251328</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G190">
     <sortCondition descending="1" ref="F2:F190"/>

</xml_diff>